<commit_message>
began creating updates for the table
</commit_message>
<xml_diff>
--- a/static/jpFlicksDoubles.xlsx
+++ b/static/jpFlicksDoubles.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C228D7D0-FCED-416B-B6E0-6CB2DB39AD73}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5490839-6AA7-4BAC-989A-7870A043D3AE}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
+    <sheet name="AwayGames" sheetId="2" r:id="rId2"/>
+    <sheet name="TeamInfo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="33">
   <si>
     <t>TGIAJF</t>
   </si>
@@ -85,13 +86,64 @@
   </si>
   <si>
     <t>Manler</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>mollyn</t>
+  </si>
+  <si>
+    <t>Katelyn</t>
+  </si>
+  <si>
+    <t>Moll Ball</t>
+  </si>
+  <si>
+    <t>Vedant</t>
+  </si>
+  <si>
+    <t>Anish</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>sam ball</t>
+  </si>
+  <si>
+    <t>kat trik</t>
+  </si>
+  <si>
+    <t>Kato</t>
+  </si>
+  <si>
+    <t>Patrik</t>
+  </si>
+  <si>
+    <t>Manu</t>
+  </si>
+  <si>
+    <t>Sandy</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +152,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -138,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,11 +205,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -170,6 +244,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,6 +268,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,14 +593,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,24 +635,51 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="9" t="str">
+        <f>IF(OR(B3 = "UNPLAYED", B3 = "XXX"), B3, -1* B3)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="D2" s="9">
+        <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <f>IF(OR(B5 = "UNPLAYED", B5 = "XXX"), B5, -1* B5)</f>
+        <v>95</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>IF(OR(B6 = "UNPLAYED", B6 = "XXX"), B6, -1* B6)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="G2" s="1">
+        <f>IF(OR(B7 = "UNPLAYED", B7 = "XXX"), B7, -1* B7)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <f>IF(OR(B8 = "UNPLAYED", B8 = "XXX"), B8, -1* B8)</f>
+        <v>55</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
+        <v>XXX</v>
+      </c>
+      <c r="J2" s="1" t="str">
+        <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
+        <v>XXX</v>
+      </c>
+      <c r="K2" s="1">
+        <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -572,16 +689,40 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="9" t="str">
+        <f>IF(OR(C4 = "UNPLAYED", C4 = "XXX"), C4, -1* C4)</f>
+        <v>XXX</v>
+      </c>
+      <c r="E3" s="9" t="str">
+        <f>IF(OR(C5 = "UNPLAYED", C5 = "XXX"), C5, -1* C5)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>IF(OR(C6 = "UNPLAYED", C6 = "XXX"), C6, -1* C6)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f>IF(OR(C7 = "UNPLAYED", C7 = "XXX"), C7, -1* C7)</f>
+        <v>XXX</v>
+      </c>
+      <c r="H3" s="1">
+        <f>IF(OR(C8 = "UNPLAYED", C8 = "XXX"), C8, -1* C8)</f>
+        <v>100</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>IF(OR(C11 = "UNPLAYED", C11 = "XXX"), C11, -1* C11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -594,15 +735,36 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="9" t="str">
+        <f>IF(OR(D5 = "UNPLAYED", D5 = "XXX"), D5, -1* D5)</f>
+        <v>XXX</v>
+      </c>
+      <c r="F4" s="9" t="str">
+        <f>IF(OR(D6 = "UNPLAYED", D6 = "XXX"), D6, -1* D6)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f>IF(OR(D7 = "UNPLAYED", D7 = "XXX"), D7, -1* D7)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f>IF(OR(D8 = "UNPLAYED", D8 = "XXX"), D8, -1* D8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f>IF(OR(D9 = "UNPLAYED", D9 = "XXX"), D9, -1* D9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J4" s="1">
+        <f>IF(OR(D10 = "UNPLAYED", D10 = "XXX"), D10, -1* D10)</f>
+        <v>65</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f>IF(OR(D11 = "UNPLAYED", D11 = "XXX"), D11, -1* D11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -618,14 +780,32 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="9" t="str">
+        <f>IF(OR(E6 = "UNPLAYED", E6 = "XXX"), E6, -1* E6)</f>
+        <v>XXX</v>
+      </c>
+      <c r="G5" s="9" t="str">
+        <f>IF(OR(E7 = "UNPLAYED", E7 = "XXX"), E7, -1* E7)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f>IF(OR(E8 = "UNPLAYED", E8 = "XXX"), E8, -1* E8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -644,13 +824,28 @@
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="9" t="str">
+        <f>IF(OR(F7 = "UNPLAYED", F7 = "XXX"), F7, -1* F7)</f>
+        <v>XXX</v>
+      </c>
+      <c r="H6" s="9" t="str">
+        <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f>IF(OR(F10 = "UNPLAYED", F10 = "XXX"), F10, -1* F10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f>IF(OR(F11 = "UNPLAYED", F11 = "XXX"), F11, -1* F11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -672,12 +867,24 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="9" t="str">
+        <f>IF(OR(G8 = "UNPLAYED", G8 = "XXX"), G8, -1* G8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I7" s="9" t="str">
+        <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -702,11 +909,20 @@
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I8" s="9">
+        <f>IF(OR(H9 = "UNPLAYED", H9 = "XXX"), H9, -1* H9)</f>
+        <v>50</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f>IF(OR(H10 = "UNPLAYED", H10 = "XXX"), H10, -1* H10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f>IF(OR(H11 = "UNPLAYED", H11 = "XXX"), H11, -1* H11)</f>
+        <v>XXX</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -734,10 +950,16 @@
       <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" s="9" t="str">
+        <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K9" s="9" t="str">
+        <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -768,9 +990,12 @@
       <c r="J10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="K10" s="9" t="str">
+        <f>IF(OR(J11 = "UNPLAYED", J11 = "XXX"), J11, -1* J11)</f>
+        <v>XXX</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -814,14 +1039,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EF8B2E-F019-48DD-B57E-84981A9F67DB}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,24 +1080,51 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="9" t="str">
+        <f>IF(OR(B3 = "UNPLAYED", B3 = "XXX"), B3, -1* B3)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="D2" s="9" t="str">
+        <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>IF(OR(B5 = "UNPLAYED", B5 = "XXX"), B5, -1* B5)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>IF(OR(B6 = "UNPLAYED", B6 = "XXX"), B6, -1* B6)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>IF(OR(B7 = "UNPLAYED", B7 = "XXX"), B7, -1* B7)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>IF(OR(B8 = "UNPLAYED", B8 = "XXX"), B8, -1* B8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
+        <v>XXX</v>
+      </c>
+      <c r="J2" s="1" t="str">
+        <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
+        <v>XXX</v>
+      </c>
+      <c r="K2" s="1">
+        <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -880,16 +1134,40 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="9" t="str">
+        <f>IF(OR(C4 = "UNPLAYED", C4 = "XXX"), C4, -1* C4)</f>
+        <v>XXX</v>
+      </c>
+      <c r="E3" s="9" t="str">
+        <f>IF(OR(C5 = "UNPLAYED", C5 = "XXX"), C5, -1* C5)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>IF(OR(C6 = "UNPLAYED", C6 = "XXX"), C6, -1* C6)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f>IF(OR(C7 = "UNPLAYED", C7 = "XXX"), C7, -1* C7)</f>
+        <v>XXX</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f>IF(OR(C8 = "UNPLAYED", C8 = "XXX"), C8, -1* C8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>IF(OR(C11 = "UNPLAYED", C11 = "XXX"), C11, -1* C11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -902,15 +1180,36 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="9" t="str">
+        <f>IF(OR(D5 = "UNPLAYED", D5 = "XXX"), D5, -1* D5)</f>
+        <v>XXX</v>
+      </c>
+      <c r="F4" s="9" t="str">
+        <f>IF(OR(D6 = "UNPLAYED", D6 = "XXX"), D6, -1* D6)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f>IF(OR(D7 = "UNPLAYED", D7 = "XXX"), D7, -1* D7)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f>IF(OR(D8 = "UNPLAYED", D8 = "XXX"), D8, -1* D8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f>IF(OR(D9 = "UNPLAYED", D9 = "XXX"), D9, -1* D9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f>IF(OR(D10 = "UNPLAYED", D10 = "XXX"), D10, -1* D10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f>IF(OR(D11 = "UNPLAYED", D11 = "XXX"), D11, -1* D11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -926,14 +1225,32 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="9" t="str">
+        <f>IF(OR(E6 = "UNPLAYED", E6 = "XXX"), E6, -1* E6)</f>
+        <v>XXX</v>
+      </c>
+      <c r="G5" s="9" t="str">
+        <f>IF(OR(E7 = "UNPLAYED", E7 = "XXX"), E7, -1* E7)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f>IF(OR(E8 = "UNPLAYED", E8 = "XXX"), E8, -1* E8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -952,13 +1269,28 @@
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="9" t="str">
+        <f>IF(OR(F7 = "UNPLAYED", F7 = "XXX"), F7, -1* F7)</f>
+        <v>XXX</v>
+      </c>
+      <c r="H6" s="9" t="str">
+        <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f>IF(OR(F10 = "UNPLAYED", F10 = "XXX"), F10, -1* F10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f>IF(OR(F11 = "UNPLAYED", F11 = "XXX"), F11, -1* F11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -980,12 +1312,24 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="9" t="str">
+        <f>IF(OR(G8 = "UNPLAYED", G8 = "XXX"), G8, -1* G8)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="I7" s="9" t="str">
+        <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1010,11 +1354,20 @@
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I8" s="9" t="str">
+        <f>IF(OR(H9 = "UNPLAYED", H9 = "XXX"), H9, -1* H9)</f>
+        <v>XXX</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f>IF(OR(H10 = "UNPLAYED", H10 = "XXX"), H10, -1* H10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f>IF(OR(H11 = "UNPLAYED", H11 = "XXX"), H11, -1* H11)</f>
+        <v>XXX</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1042,10 +1395,16 @@
       <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" s="9" t="str">
+        <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K9" s="9" t="str">
+        <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1076,9 +1435,12 @@
       <c r="J10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="K10" s="9" t="str">
+        <f>IF(OR(J11 = "UNPLAYED", J11 = "XXX"), J11, -1* J11)</f>
+        <v>XXX</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1111,6 +1473,142 @@
       </c>
       <c r="K11" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F4B8BC-1389-42AE-87D2-D523A6E6AA2A}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed game finder table
</commit_message>
<xml_diff>
--- a/static/jpFlicksDoubles.xlsx
+++ b/static/jpFlicksDoubles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{725FC128-B5EB-4100-98A1-E7CFF211783A}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB86F4D9-547C-48F9-A589-637DD80AF05C}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
   <si>
     <t>TGIAJF</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Sam</t>
-  </si>
-  <si>
-    <t>kat trik</t>
   </si>
   <si>
     <t>Kato</t>
@@ -578,18 +575,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -607,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -622,7 +619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,7 +706,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -751,7 +748,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -792,7 +789,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,9 +829,9 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5">
         <v>0</v>
@@ -871,7 +868,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -909,7 +906,7 @@
         <v>XXX</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -946,7 +943,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -982,7 +979,7 @@
         <v>XXX</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1026,15 +1023,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EF8B2E-F019-48DD-B57E-84981A9F67DB}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1052,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1067,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1108,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1151,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1237,7 +1234,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1277,9 +1274,9 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -1316,7 +1313,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1354,7 +1351,7 @@
         <v>XXX</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1391,7 +1388,7 @@
         <v>UNPLAYED</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1427,7 +1424,7 @@
         <v>XXX</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1472,14 +1469,14 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>11</v>
@@ -1488,7 +1485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1510,7 +1507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1521,7 +1518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1532,7 +1529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1543,9 +1540,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>16</v>
@@ -1554,18 +1551,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -1573,29 +1570,29 @@
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>